<commit_message>
Fixed a few minor bugs
</commit_message>
<xml_diff>
--- a/outputs/output_template.xlsx
+++ b/outputs/output_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luish\Documents\Repos\Trading algorithms\trunk\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4981001-23F0-4A25-A116-80BDB4C6E2F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED588F84-90F3-4459-A13D-D1D885F52649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Execution" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3064"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -9820,6 +9820,7 @@
     <col min="12" max="12" width="13.1796875" style="15" customWidth="1"/>
     <col min="13" max="13" width="12.26953125" style="15" customWidth="1"/>
     <col min="14" max="14" width="12" style="16" customWidth="1"/>
+    <col min="15" max="37" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -11074,7 +11075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added option to only use one open position
</commit_message>
<xml_diff>
--- a/outputs/output_template.xlsx
+++ b/outputs/output_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luish\Documents\Repos\Trading algorithms\trunk\outputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED588F84-90F3-4459-A13D-D1D885F52649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DB4991-E328-4762-8A23-CB6815974024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Execution" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Parameters" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backtesting!$A$7:$N$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Backtesting!$A$7:$R$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Execution!$A$7:$H$7</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Optimization!$A$7:$N$7</definedName>
   </definedNames>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="26">
   <si>
     <t>python</t>
   </si>
@@ -118,6 +118,9 @@
   <si>
     <t>Amount exit
 (EUR)</t>
+  </si>
+  <si>
+    <t>Profit/Loss Cum (EUR)</t>
   </si>
 </sst>
 </file>
@@ -496,9 +499,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3064"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9800,7 +9803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R123"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -9820,7 +9823,8 @@
     <col min="12" max="12" width="13.1796875" style="15" customWidth="1"/>
     <col min="13" max="13" width="12.26953125" style="15" customWidth="1"/>
     <col min="14" max="14" width="12" style="16" customWidth="1"/>
-    <col min="15" max="37" width="16.6328125" customWidth="1"/>
+    <col min="15" max="15" width="15.6328125" customWidth="1"/>
+    <col min="16" max="37" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -9908,6 +9912,611 @@
       <c r="L5"/>
       <c r="M5"/>
       <c r="N5"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G8" s="14"/>
+      <c r="I8" s="14"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G9" s="14"/>
+      <c r="I9" s="14"/>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G10" s="14"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G11" s="14"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G12" s="14"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G13" s="14"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G14" s="14"/>
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G15" s="14"/>
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="G16" s="14"/>
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G17" s="14"/>
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G18" s="14"/>
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G19" s="14"/>
+      <c r="I19" s="14"/>
+    </row>
+    <row r="20" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G20" s="14"/>
+      <c r="I20" s="14"/>
+    </row>
+    <row r="21" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G21" s="14"/>
+      <c r="I21" s="14"/>
+    </row>
+    <row r="22" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G22" s="14"/>
+      <c r="I22" s="14"/>
+    </row>
+    <row r="23" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G23" s="14"/>
+      <c r="I23" s="14"/>
+    </row>
+    <row r="24" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G24" s="14"/>
+      <c r="I24" s="14"/>
+    </row>
+    <row r="25" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G25" s="14"/>
+      <c r="I25" s="14"/>
+    </row>
+    <row r="26" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G26" s="14"/>
+      <c r="I26" s="14"/>
+    </row>
+    <row r="27" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G27" s="14"/>
+      <c r="I27" s="14"/>
+    </row>
+    <row r="28" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G28" s="14"/>
+      <c r="I28" s="14"/>
+    </row>
+    <row r="29" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G29" s="14"/>
+      <c r="I29" s="14"/>
+    </row>
+    <row r="30" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G30" s="14"/>
+      <c r="I30" s="14"/>
+    </row>
+    <row r="31" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G31" s="14"/>
+      <c r="I31" s="14"/>
+    </row>
+    <row r="32" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G32" s="14"/>
+      <c r="I32" s="14"/>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G33" s="14"/>
+      <c r="I33" s="14"/>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G34" s="14"/>
+      <c r="I34" s="14"/>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G35" s="14"/>
+      <c r="I35" s="14"/>
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G36" s="14"/>
+      <c r="I36" s="14"/>
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G37" s="14"/>
+      <c r="I37" s="14"/>
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G38" s="14"/>
+      <c r="I38" s="14"/>
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G39" s="14"/>
+      <c r="I39" s="14"/>
+    </row>
+    <row r="40" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G40" s="14"/>
+      <c r="I40" s="14"/>
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G41" s="14"/>
+      <c r="I41" s="14"/>
+    </row>
+    <row r="42" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G42" s="14"/>
+      <c r="I42" s="14"/>
+    </row>
+    <row r="43" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G43" s="14"/>
+      <c r="I43" s="14"/>
+    </row>
+    <row r="44" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G44" s="14"/>
+      <c r="I44" s="14"/>
+    </row>
+    <row r="45" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G45" s="14"/>
+      <c r="I45" s="14"/>
+    </row>
+    <row r="46" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G46" s="14"/>
+      <c r="I46" s="14"/>
+    </row>
+    <row r="47" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G47" s="14"/>
+      <c r="I47" s="14"/>
+    </row>
+    <row r="48" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G48" s="14"/>
+      <c r="I48" s="14"/>
+    </row>
+    <row r="49" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G49" s="14"/>
+      <c r="I49" s="14"/>
+    </row>
+    <row r="50" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G50" s="14"/>
+      <c r="I50" s="14"/>
+    </row>
+    <row r="51" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G51" s="14"/>
+      <c r="I51" s="14"/>
+    </row>
+    <row r="52" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G52" s="14"/>
+      <c r="I52" s="14"/>
+    </row>
+    <row r="53" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G53" s="14"/>
+      <c r="I53" s="14"/>
+    </row>
+    <row r="54" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G54" s="14"/>
+      <c r="I54" s="14"/>
+    </row>
+    <row r="55" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G55" s="14"/>
+      <c r="I55" s="14"/>
+    </row>
+    <row r="56" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G56" s="14"/>
+      <c r="I56" s="14"/>
+    </row>
+    <row r="57" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G57" s="14"/>
+      <c r="I57" s="14"/>
+    </row>
+    <row r="58" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G58" s="14"/>
+      <c r="I58" s="14"/>
+    </row>
+    <row r="59" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G59" s="14"/>
+      <c r="I59" s="14"/>
+    </row>
+    <row r="60" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G60" s="14"/>
+      <c r="I60" s="14"/>
+    </row>
+    <row r="61" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G61" s="14"/>
+      <c r="I61" s="14"/>
+    </row>
+    <row r="62" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G62" s="14"/>
+      <c r="I62" s="14"/>
+    </row>
+    <row r="63" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G63" s="14"/>
+      <c r="I63" s="14"/>
+    </row>
+    <row r="64" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G64" s="14"/>
+      <c r="I64" s="14"/>
+    </row>
+    <row r="65" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G65" s="14"/>
+      <c r="I65" s="14"/>
+    </row>
+    <row r="66" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G66" s="14"/>
+      <c r="I66" s="14"/>
+    </row>
+    <row r="67" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G67" s="14"/>
+      <c r="I67" s="14"/>
+    </row>
+    <row r="68" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G68" s="14"/>
+      <c r="I68" s="14"/>
+    </row>
+    <row r="69" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G69" s="14"/>
+      <c r="I69" s="14"/>
+    </row>
+    <row r="70" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G70" s="14"/>
+      <c r="I70" s="14"/>
+    </row>
+    <row r="71" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G71" s="14"/>
+      <c r="I71" s="14"/>
+    </row>
+    <row r="72" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G72" s="14"/>
+      <c r="I72" s="14"/>
+    </row>
+    <row r="73" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G73" s="14"/>
+      <c r="I73" s="14"/>
+    </row>
+    <row r="74" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G74" s="14"/>
+      <c r="I74" s="14"/>
+    </row>
+    <row r="75" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G75" s="14"/>
+      <c r="I75" s="14"/>
+    </row>
+    <row r="76" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G76" s="14"/>
+      <c r="I76" s="14"/>
+    </row>
+    <row r="77" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G77" s="14"/>
+      <c r="I77" s="14"/>
+    </row>
+    <row r="78" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G78" s="14"/>
+      <c r="I78" s="14"/>
+    </row>
+    <row r="79" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G79" s="14"/>
+      <c r="I79" s="14"/>
+    </row>
+    <row r="80" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G80" s="14"/>
+      <c r="I80" s="14"/>
+    </row>
+    <row r="81" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G81" s="14"/>
+      <c r="I81" s="14"/>
+    </row>
+    <row r="82" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G82" s="14"/>
+      <c r="I82" s="14"/>
+    </row>
+    <row r="83" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G83" s="14"/>
+      <c r="I83" s="14"/>
+    </row>
+    <row r="84" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G84" s="14"/>
+      <c r="I84" s="14"/>
+    </row>
+    <row r="85" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G85" s="14"/>
+      <c r="I85" s="14"/>
+    </row>
+    <row r="86" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G86" s="14"/>
+      <c r="I86" s="14"/>
+    </row>
+    <row r="87" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G87" s="14"/>
+      <c r="I87" s="14"/>
+    </row>
+    <row r="88" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G88" s="14"/>
+      <c r="I88" s="14"/>
+    </row>
+    <row r="89" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G89" s="14"/>
+      <c r="I89" s="14"/>
+    </row>
+    <row r="90" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G90" s="14"/>
+      <c r="I90" s="14"/>
+    </row>
+    <row r="91" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G91" s="14"/>
+      <c r="I91" s="14"/>
+    </row>
+    <row r="92" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G92" s="14"/>
+      <c r="I92" s="14"/>
+    </row>
+    <row r="93" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G93" s="14"/>
+      <c r="I93" s="14"/>
+    </row>
+    <row r="94" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G94" s="14"/>
+      <c r="I94" s="14"/>
+    </row>
+    <row r="95" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G95" s="14"/>
+      <c r="I95" s="14"/>
+    </row>
+    <row r="96" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G96" s="14"/>
+      <c r="I96" s="14"/>
+    </row>
+    <row r="97" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G97" s="14"/>
+      <c r="I97" s="14"/>
+    </row>
+    <row r="98" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G98" s="14"/>
+      <c r="I98" s="14"/>
+    </row>
+    <row r="99" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G99" s="14"/>
+      <c r="I99" s="14"/>
+    </row>
+    <row r="100" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G100" s="14"/>
+      <c r="I100" s="14"/>
+    </row>
+    <row r="101" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G101" s="14"/>
+      <c r="I101" s="14"/>
+    </row>
+    <row r="102" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G102" s="14"/>
+      <c r="I102" s="14"/>
+    </row>
+    <row r="103" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G103" s="14"/>
+      <c r="I103" s="14"/>
+    </row>
+    <row r="104" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G104" s="14"/>
+      <c r="I104" s="14"/>
+    </row>
+    <row r="105" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G105" s="14"/>
+      <c r="I105" s="14"/>
+    </row>
+    <row r="106" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G106" s="14"/>
+      <c r="I106" s="14"/>
+    </row>
+    <row r="107" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G107" s="14"/>
+      <c r="I107" s="14"/>
+    </row>
+    <row r="108" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G108" s="14"/>
+      <c r="I108" s="14"/>
+    </row>
+    <row r="109" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G109" s="14"/>
+      <c r="I109" s="14"/>
+    </row>
+    <row r="110" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G110" s="14"/>
+      <c r="I110" s="14"/>
+    </row>
+    <row r="111" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G111" s="14"/>
+      <c r="I111" s="14"/>
+    </row>
+    <row r="112" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G112" s="14"/>
+      <c r="I112" s="14"/>
+    </row>
+    <row r="113" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G113" s="14"/>
+      <c r="I113" s="14"/>
+    </row>
+    <row r="114" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G114" s="14"/>
+      <c r="I114" s="14"/>
+    </row>
+    <row r="115" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G115" s="14"/>
+      <c r="I115" s="14"/>
+    </row>
+    <row r="116" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G116" s="14"/>
+      <c r="I116" s="14"/>
+    </row>
+    <row r="117" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G117" s="14"/>
+      <c r="I117" s="14"/>
+    </row>
+    <row r="118" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G118" s="14"/>
+      <c r="I118" s="14"/>
+    </row>
+    <row r="119" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G119" s="14"/>
+      <c r="I119" s="14"/>
+    </row>
+    <row r="120" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G120" s="14"/>
+      <c r="I120" s="14"/>
+    </row>
+    <row r="121" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G121" s="14"/>
+      <c r="I121" s="14"/>
+    </row>
+    <row r="122" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G122" s="14"/>
+      <c r="I122" s="14"/>
+    </row>
+    <row r="123" spans="7:9" x14ac:dyDescent="0.35">
+      <c r="G123" s="14"/>
+      <c r="I123" s="14"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A7:R7" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8EA595-09D3-4FF5-B36C-A6CA7B8ED474}">
+  <dimension ref="A1:R123"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.26953125" customWidth="1"/>
+    <col min="3" max="4" width="12" customWidth="1"/>
+    <col min="7" max="7" width="16.7265625" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" customWidth="1"/>
+    <col min="9" max="9" width="14.1796875" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" customWidth="1"/>
+    <col min="11" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="13.1796875" customWidth="1"/>
+    <col min="13" max="13" width="12.26953125" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -10002,606 +10611,6 @@
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="G8" s="14"/>
-      <c r="I8" s="14"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="G9" s="14"/>
-      <c r="I9" s="14"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="G10" s="14"/>
-      <c r="I10" s="14"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="G11" s="14"/>
-      <c r="I11" s="14"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="G12" s="14"/>
-      <c r="I12" s="14"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="G13" s="14"/>
-      <c r="I13" s="14"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="G14" s="14"/>
-      <c r="I14" s="14"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="G15" s="14"/>
-      <c r="I15" s="14"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="G16" s="14"/>
-      <c r="I16" s="14"/>
-    </row>
-    <row r="17" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G17" s="14"/>
-      <c r="I17" s="14"/>
-    </row>
-    <row r="18" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G18" s="14"/>
-      <c r="I18" s="14"/>
-    </row>
-    <row r="19" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G19" s="14"/>
-      <c r="I19" s="14"/>
-    </row>
-    <row r="20" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G20" s="14"/>
-      <c r="I20" s="14"/>
-    </row>
-    <row r="21" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G21" s="14"/>
-      <c r="I21" s="14"/>
-    </row>
-    <row r="22" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G22" s="14"/>
-      <c r="I22" s="14"/>
-    </row>
-    <row r="23" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G23" s="14"/>
-      <c r="I23" s="14"/>
-    </row>
-    <row r="24" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G24" s="14"/>
-      <c r="I24" s="14"/>
-    </row>
-    <row r="25" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G25" s="14"/>
-      <c r="I25" s="14"/>
-    </row>
-    <row r="26" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G26" s="14"/>
-      <c r="I26" s="14"/>
-    </row>
-    <row r="27" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G27" s="14"/>
-      <c r="I27" s="14"/>
-    </row>
-    <row r="28" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G28" s="14"/>
-      <c r="I28" s="14"/>
-    </row>
-    <row r="29" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G29" s="14"/>
-      <c r="I29" s="14"/>
-    </row>
-    <row r="30" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G30" s="14"/>
-      <c r="I30" s="14"/>
-    </row>
-    <row r="31" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G31" s="14"/>
-      <c r="I31" s="14"/>
-    </row>
-    <row r="32" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G32" s="14"/>
-      <c r="I32" s="14"/>
-    </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G33" s="14"/>
-      <c r="I33" s="14"/>
-    </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G34" s="14"/>
-      <c r="I34" s="14"/>
-    </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G35" s="14"/>
-      <c r="I35" s="14"/>
-    </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G36" s="14"/>
-      <c r="I36" s="14"/>
-    </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G37" s="14"/>
-      <c r="I37" s="14"/>
-    </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G38" s="14"/>
-      <c r="I38" s="14"/>
-    </row>
-    <row r="39" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G39" s="14"/>
-      <c r="I39" s="14"/>
-    </row>
-    <row r="40" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G40" s="14"/>
-      <c r="I40" s="14"/>
-    </row>
-    <row r="41" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G41" s="14"/>
-      <c r="I41" s="14"/>
-    </row>
-    <row r="42" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G42" s="14"/>
-      <c r="I42" s="14"/>
-    </row>
-    <row r="43" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G43" s="14"/>
-      <c r="I43" s="14"/>
-    </row>
-    <row r="44" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G44" s="14"/>
-      <c r="I44" s="14"/>
-    </row>
-    <row r="45" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G45" s="14"/>
-      <c r="I45" s="14"/>
-    </row>
-    <row r="46" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G46" s="14"/>
-      <c r="I46" s="14"/>
-    </row>
-    <row r="47" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G47" s="14"/>
-      <c r="I47" s="14"/>
-    </row>
-    <row r="48" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G48" s="14"/>
-      <c r="I48" s="14"/>
-    </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G49" s="14"/>
-      <c r="I49" s="14"/>
-    </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G50" s="14"/>
-      <c r="I50" s="14"/>
-    </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G51" s="14"/>
-      <c r="I51" s="14"/>
-    </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G52" s="14"/>
-      <c r="I52" s="14"/>
-    </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G53" s="14"/>
-      <c r="I53" s="14"/>
-    </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G54" s="14"/>
-      <c r="I54" s="14"/>
-    </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G55" s="14"/>
-      <c r="I55" s="14"/>
-    </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G56" s="14"/>
-      <c r="I56" s="14"/>
-    </row>
-    <row r="57" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G57" s="14"/>
-      <c r="I57" s="14"/>
-    </row>
-    <row r="58" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G58" s="14"/>
-      <c r="I58" s="14"/>
-    </row>
-    <row r="59" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G59" s="14"/>
-      <c r="I59" s="14"/>
-    </row>
-    <row r="60" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G60" s="14"/>
-      <c r="I60" s="14"/>
-    </row>
-    <row r="61" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G61" s="14"/>
-      <c r="I61" s="14"/>
-    </row>
-    <row r="62" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G62" s="14"/>
-      <c r="I62" s="14"/>
-    </row>
-    <row r="63" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G63" s="14"/>
-      <c r="I63" s="14"/>
-    </row>
-    <row r="64" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G64" s="14"/>
-      <c r="I64" s="14"/>
-    </row>
-    <row r="65" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G65" s="14"/>
-      <c r="I65" s="14"/>
-    </row>
-    <row r="66" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G66" s="14"/>
-      <c r="I66" s="14"/>
-    </row>
-    <row r="67" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G67" s="14"/>
-      <c r="I67" s="14"/>
-    </row>
-    <row r="68" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G68" s="14"/>
-      <c r="I68" s="14"/>
-    </row>
-    <row r="69" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G69" s="14"/>
-      <c r="I69" s="14"/>
-    </row>
-    <row r="70" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G70" s="14"/>
-      <c r="I70" s="14"/>
-    </row>
-    <row r="71" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G71" s="14"/>
-      <c r="I71" s="14"/>
-    </row>
-    <row r="72" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G72" s="14"/>
-      <c r="I72" s="14"/>
-    </row>
-    <row r="73" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G73" s="14"/>
-      <c r="I73" s="14"/>
-    </row>
-    <row r="74" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G74" s="14"/>
-      <c r="I74" s="14"/>
-    </row>
-    <row r="75" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G75" s="14"/>
-      <c r="I75" s="14"/>
-    </row>
-    <row r="76" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G76" s="14"/>
-      <c r="I76" s="14"/>
-    </row>
-    <row r="77" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G77" s="14"/>
-      <c r="I77" s="14"/>
-    </row>
-    <row r="78" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G78" s="14"/>
-      <c r="I78" s="14"/>
-    </row>
-    <row r="79" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G79" s="14"/>
-      <c r="I79" s="14"/>
-    </row>
-    <row r="80" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G80" s="14"/>
-      <c r="I80" s="14"/>
-    </row>
-    <row r="81" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G81" s="14"/>
-      <c r="I81" s="14"/>
-    </row>
-    <row r="82" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G82" s="14"/>
-      <c r="I82" s="14"/>
-    </row>
-    <row r="83" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G83" s="14"/>
-      <c r="I83" s="14"/>
-    </row>
-    <row r="84" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G84" s="14"/>
-      <c r="I84" s="14"/>
-    </row>
-    <row r="85" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G85" s="14"/>
-      <c r="I85" s="14"/>
-    </row>
-    <row r="86" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G86" s="14"/>
-      <c r="I86" s="14"/>
-    </row>
-    <row r="87" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G87" s="14"/>
-      <c r="I87" s="14"/>
-    </row>
-    <row r="88" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G88" s="14"/>
-      <c r="I88" s="14"/>
-    </row>
-    <row r="89" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G89" s="14"/>
-      <c r="I89" s="14"/>
-    </row>
-    <row r="90" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G90" s="14"/>
-      <c r="I90" s="14"/>
-    </row>
-    <row r="91" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G91" s="14"/>
-      <c r="I91" s="14"/>
-    </row>
-    <row r="92" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G92" s="14"/>
-      <c r="I92" s="14"/>
-    </row>
-    <row r="93" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G93" s="14"/>
-      <c r="I93" s="14"/>
-    </row>
-    <row r="94" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G94" s="14"/>
-      <c r="I94" s="14"/>
-    </row>
-    <row r="95" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G95" s="14"/>
-      <c r="I95" s="14"/>
-    </row>
-    <row r="96" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G96" s="14"/>
-      <c r="I96" s="14"/>
-    </row>
-    <row r="97" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G97" s="14"/>
-      <c r="I97" s="14"/>
-    </row>
-    <row r="98" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G98" s="14"/>
-      <c r="I98" s="14"/>
-    </row>
-    <row r="99" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G99" s="14"/>
-      <c r="I99" s="14"/>
-    </row>
-    <row r="100" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G100" s="14"/>
-      <c r="I100" s="14"/>
-    </row>
-    <row r="101" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G101" s="14"/>
-      <c r="I101" s="14"/>
-    </row>
-    <row r="102" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G102" s="14"/>
-      <c r="I102" s="14"/>
-    </row>
-    <row r="103" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G103" s="14"/>
-      <c r="I103" s="14"/>
-    </row>
-    <row r="104" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G104" s="14"/>
-      <c r="I104" s="14"/>
-    </row>
-    <row r="105" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G105" s="14"/>
-      <c r="I105" s="14"/>
-    </row>
-    <row r="106" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G106" s="14"/>
-      <c r="I106" s="14"/>
-    </row>
-    <row r="107" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G107" s="14"/>
-      <c r="I107" s="14"/>
-    </row>
-    <row r="108" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G108" s="14"/>
-      <c r="I108" s="14"/>
-    </row>
-    <row r="109" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G109" s="14"/>
-      <c r="I109" s="14"/>
-    </row>
-    <row r="110" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G110" s="14"/>
-      <c r="I110" s="14"/>
-    </row>
-    <row r="111" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G111" s="14"/>
-      <c r="I111" s="14"/>
-    </row>
-    <row r="112" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G112" s="14"/>
-      <c r="I112" s="14"/>
-    </row>
-    <row r="113" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G113" s="14"/>
-      <c r="I113" s="14"/>
-    </row>
-    <row r="114" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G114" s="14"/>
-      <c r="I114" s="14"/>
-    </row>
-    <row r="115" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G115" s="14"/>
-      <c r="I115" s="14"/>
-    </row>
-    <row r="116" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G116" s="14"/>
-      <c r="I116" s="14"/>
-    </row>
-    <row r="117" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G117" s="14"/>
-      <c r="I117" s="14"/>
-    </row>
-    <row r="118" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G118" s="14"/>
-      <c r="I118" s="14"/>
-    </row>
-    <row r="119" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G119" s="14"/>
-      <c r="I119" s="14"/>
-    </row>
-    <row r="120" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G120" s="14"/>
-      <c r="I120" s="14"/>
-    </row>
-    <row r="121" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G121" s="14"/>
-      <c r="I121" s="14"/>
-    </row>
-    <row r="122" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G122" s="14"/>
-      <c r="I122" s="14"/>
-    </row>
-    <row r="123" spans="7:9" x14ac:dyDescent="0.35">
-      <c r="G123" s="14"/>
-      <c r="I123" s="14"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A7:N7" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8EA595-09D3-4FF5-B36C-A6CA7B8ED474}">
-  <dimension ref="A1:R123"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="15.26953125" customWidth="1"/>
-    <col min="3" max="4" width="12" customWidth="1"/>
-    <col min="7" max="7" width="16.7265625" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" customWidth="1"/>
-    <col min="9" max="9" width="14.1796875" customWidth="1"/>
-    <col min="10" max="10" width="11.54296875" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="13.1796875" customWidth="1"/>
-    <col min="13" max="13" width="12.26953125" customWidth="1"/>
-    <col min="14" max="14" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
-        <v>0</v>
-      </c>
-      <c r="M6" t="s">
-        <v>0</v>
-      </c>
-      <c r="N6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="G8" s="8"/>
       <c r="I8" s="8"/>
     </row>

</xml_diff>